<commit_message>
Added temp reqs and fuse values
</commit_message>
<xml_diff>
--- a/Loom23/Loomwires.xlsx
+++ b/Loom23/Loomwires.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/fst29_cam_ac_uk/Documents/SF/fbr20-electronics/Loom23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ifs.eng.cam.ac.uk\users\fst29\Documents\Loom23\Loom23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="628" documentId="11_F25DC773A252ABDACC104812991E59BC5ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B678C150-4D7C-4893-A0CF-6868FB76F223}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23236D3A-2752-444C-B7A2-22186F4803D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="220">
   <si>
     <t>Label</t>
   </si>
@@ -683,9 +680,6 @@
     <t>100A</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>15A</t>
   </si>
   <si>
@@ -696,6 +690,9 @@
   </si>
   <si>
     <t>82A</t>
+  </si>
+  <si>
+    <t>Yes, needs label</t>
   </si>
 </sst>
 </file>
@@ -731,9 +728,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1022,61 +1022,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="106.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1107,13 +1107,13 @@
       <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1135,8 +1135,11 @@
       <c r="M3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1660,8 +1663,11 @@
       <c r="M21" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N21" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1707,7 +1713,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1753,7 +1759,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -1844,8 +1850,20 @@
       <c r="L29" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>207</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>197</v>
       </c>
@@ -1874,7 +1892,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>198</v>
       </c>
@@ -1903,7 +1921,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1926,7 +1944,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1949,7 +1967,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1972,7 +1990,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2001,7 +2019,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2020,8 +2038,14 @@
       <c r="L36" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>203</v>
+      </c>
+      <c r="N36" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2043,8 +2067,11 @@
       <c r="M37" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2063,8 +2090,14 @@
       <c r="L38" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M38" t="s">
+        <v>203</v>
+      </c>
+      <c r="N38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2086,11 +2119,14 @@
       <c r="M39" t="s">
         <v>211</v>
       </c>
+      <c r="N39" t="s">
+        <v>204</v>
+      </c>
       <c r="O39" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2112,8 +2148,11 @@
       <c r="M40" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N40" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2145,10 +2184,10 @@
         <v>171</v>
       </c>
       <c r="M41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -2171,7 +2210,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2190,8 +2229,11 @@
       <c r="L43" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M43" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2213,11 +2255,14 @@
       <c r="M44" t="s">
         <v>203</v>
       </c>
+      <c r="N44" t="s">
+        <v>204</v>
+      </c>
       <c r="O44" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -2257,11 +2302,14 @@
       <c r="M45" t="s">
         <v>213</v>
       </c>
+      <c r="N45" t="s">
+        <v>204</v>
+      </c>
       <c r="O45" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2280,11 +2328,14 @@
       <c r="L46" t="s">
         <v>176</v>
       </c>
+      <c r="M46" t="s">
+        <v>203</v>
+      </c>
       <c r="O46" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2310,7 +2361,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2329,11 +2380,14 @@
       <c r="L48" t="s">
         <v>177</v>
       </c>
+      <c r="M48" t="s">
+        <v>203</v>
+      </c>
       <c r="O48" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2356,7 +2410,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2378,8 +2432,11 @@
       <c r="M50" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2401,8 +2458,11 @@
       <c r="M51" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2424,8 +2484,11 @@
       <c r="M52" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2444,8 +2507,11 @@
       <c r="L53" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O53" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2464,8 +2530,11 @@
       <c r="L54" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O54" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2491,7 +2560,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2517,7 +2586,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2536,8 +2605,11 @@
       <c r="L57" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M57" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2560,10 +2632,10 @@
         <v>214</v>
       </c>
       <c r="O58" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2586,10 +2658,10 @@
         <v>214</v>
       </c>
       <c r="O59" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2609,10 +2681,10 @@
         <v>188</v>
       </c>
       <c r="M60" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2632,10 +2704,10 @@
         <v>189</v>
       </c>
       <c r="M61" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2652,13 +2724,13 @@
         <v>75</v>
       </c>
       <c r="L62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M62" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2681,7 +2753,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2704,7 +2776,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2727,7 +2799,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2747,7 +2819,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2764,7 +2836,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2784,7 +2856,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2806,8 +2878,11 @@
       <c r="M69" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2826,8 +2901,11 @@
       <c r="M70" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N70" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2843,8 +2921,11 @@
       <c r="M71" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N71" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2862,6 +2943,9 @@
       </c>
       <c r="M72" t="s">
         <v>203</v>
+      </c>
+      <c r="N72" t="s">
+        <v>204</v>
       </c>
       <c r="O72" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
Added paddle shifter PCB and the relays.
</commit_message>
<xml_diff>
--- a/Loom23/Loomwires.xlsx
+++ b/Loom23/Loomwires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/fst29_cam_ac_uk/Documents/SF/fbr20-electronics/Loom23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ifs.eng.cam.ac.uk\users\fst29\Documents\Loom23\fbr20-electronics\Loom23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{23236D3A-2752-444C-B7A2-22186F4803D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA88E3BA-4EC7-4B9D-AD75-81925D3654D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09F1BC-7B75-4486-AC42-630B9AE639E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="244">
   <si>
     <t>Label</t>
   </si>
@@ -714,6 +706,57 @@
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>ShifterPressure</t>
+  </si>
+  <si>
+    <t>SwitchSolenoid</t>
+  </si>
+  <si>
+    <t>UpSolenoid</t>
+  </si>
+  <si>
+    <t>DownSolenoid</t>
+  </si>
+  <si>
+    <t>ShifterPump</t>
+  </si>
+  <si>
+    <t>NeutralSensor</t>
+  </si>
+  <si>
+    <t>Neutral Sensor</t>
+  </si>
+  <si>
+    <t>Signal of the neutral sensor on the engine</t>
+  </si>
+  <si>
+    <t>Gearbox  pneumatics</t>
+  </si>
+  <si>
+    <t>Output to solenoid on down shift valve</t>
+  </si>
+  <si>
+    <t>Output to solenoid on up shift valve</t>
+  </si>
+  <si>
+    <t>Output to switch solenoid used to start pump from atmosphere</t>
+  </si>
+  <si>
+    <t>High current pump output</t>
+  </si>
+  <si>
+    <t>Analog input from pneumatic pressure sensor</t>
+  </si>
+  <si>
+    <t>0.5A</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>Wires in the dash area are still very much WIP.</t>
   </si>
 </sst>
 </file>
@@ -749,18 +792,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,80 +1085,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="100.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="100.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1145,15 +1189,15 @@
       <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1182,7 +1226,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1220,7 +1264,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1302,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -1293,7 +1337,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -1328,7 +1372,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1363,7 +1407,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1395,7 +1439,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1421,7 +1465,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1447,7 +1491,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1473,7 +1517,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1505,7 +1549,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1537,7 +1581,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1566,7 +1610,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1595,7 +1639,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1630,7 +1674,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1665,7 +1709,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1700,7 +1744,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +1788,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1773,7 +1817,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1799,7 +1843,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1825,7 +1869,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1851,7 +1895,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1877,7 +1921,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1903,7 +1947,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1929,7 +1973,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1961,7 +2005,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -1996,7 +2040,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>197</v>
       </c>
@@ -2031,7 +2075,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>198</v>
       </c>
@@ -2066,7 +2110,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2088,11 +2132,11 @@
       <c r="M32" t="s">
         <v>203</v>
       </c>
-      <c r="Q32" s="4" t="s">
+      <c r="Q32" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2114,11 +2158,11 @@
       <c r="M33" t="s">
         <v>203</v>
       </c>
-      <c r="Q33" s="4" t="s">
+      <c r="Q33" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2140,11 +2184,11 @@
       <c r="M34" t="s">
         <v>203</v>
       </c>
-      <c r="Q34" s="4" t="s">
+      <c r="Q34" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2176,7 +2220,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2202,7 +2246,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2228,7 +2272,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2254,7 +2298,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2283,7 +2327,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2309,7 +2353,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2344,7 +2388,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -2367,7 +2411,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2390,7 +2434,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2419,7 +2463,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
@@ -2466,7 +2510,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2492,7 +2536,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2518,7 +2562,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2544,7 +2588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2567,7 +2611,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2593,7 +2637,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2619,7 +2663,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2645,7 +2689,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2668,7 +2712,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2691,7 +2735,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2717,7 +2761,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2743,7 +2787,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2766,7 +2810,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2792,7 +2836,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2818,7 +2862,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2841,7 +2885,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2864,7 +2908,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2887,7 +2931,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2910,7 +2954,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2933,7 +2977,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2956,7 +3000,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2979,7 +3023,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3002,7 +3046,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3022,7 +3066,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3048,7 +3092,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3071,7 +3115,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3091,7 +3135,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3115,6 +3159,167 @@
       </c>
       <c r="O72" t="s">
         <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>227</v>
+      </c>
+      <c r="B73" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="5">
+        <v>14</v>
+      </c>
+      <c r="D73" t="s">
+        <v>235</v>
+      </c>
+      <c r="E73" t="s">
+        <v>75</v>
+      </c>
+      <c r="L73" t="s">
+        <v>240</v>
+      </c>
+      <c r="M73" t="s">
+        <v>203</v>
+      </c>
+      <c r="O73" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>228</v>
+      </c>
+      <c r="B74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>235</v>
+      </c>
+      <c r="E74" t="s">
+        <v>75</v>
+      </c>
+      <c r="L74" t="s">
+        <v>238</v>
+      </c>
+      <c r="M74" t="s">
+        <v>241</v>
+      </c>
+      <c r="O74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>229</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>235</v>
+      </c>
+      <c r="E75" t="s">
+        <v>75</v>
+      </c>
+      <c r="L75" t="s">
+        <v>237</v>
+      </c>
+      <c r="M75" t="s">
+        <v>241</v>
+      </c>
+      <c r="O75" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>235</v>
+      </c>
+      <c r="E76" t="s">
+        <v>75</v>
+      </c>
+      <c r="L76" t="s">
+        <v>236</v>
+      </c>
+      <c r="M76" t="s">
+        <v>241</v>
+      </c>
+      <c r="O76" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>231</v>
+      </c>
+      <c r="B77" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>235</v>
+      </c>
+      <c r="E77" t="s">
+        <v>75</v>
+      </c>
+      <c r="L77" t="s">
+        <v>239</v>
+      </c>
+      <c r="M77" t="s">
+        <v>242</v>
+      </c>
+      <c r="O77" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78">
+        <v>13</v>
+      </c>
+      <c r="D78" t="s">
+        <v>233</v>
+      </c>
+      <c r="E78" t="s">
+        <v>75</v>
+      </c>
+      <c r="L78" t="s">
+        <v>234</v>
+      </c>
+      <c r="M78" t="s">
+        <v>203</v>
+      </c>
+      <c r="O78" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed labels to match in schematic and spreadsheet
</commit_message>
<xml_diff>
--- a/Loom23/Loomwires.xlsx
+++ b/Loom23/Loomwires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/fst29_cam_ac_uk/Documents/SF/fbr20-electronics/Loom23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{C4FF7FE4-E9F4-478E-AFE7-68957E8D9EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB702788-C242-4A9A-AED5-8B186BAE37EF}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{C4FF7FE4-E9F4-478E-AFE7-68957E8D9EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{326B12D1-0538-4ACC-B01A-9E02DAEB7050}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="251">
   <si>
     <t>Label</t>
   </si>
@@ -594,9 +594,6 @@
     <t>Square wave ignition signal input, not used</t>
   </si>
   <si>
-    <t>VR2IN+</t>
-  </si>
-  <si>
     <t>Not used</t>
   </si>
   <si>
@@ -705,9 +702,6 @@
     <t>Brake Line pressure sensor</t>
   </si>
   <si>
-    <t>Brake Light</t>
-  </si>
-  <si>
     <t>Brake light</t>
   </si>
   <si>
@@ -750,12 +744,6 @@
     <t>Yes, needs heatshring</t>
   </si>
   <si>
-    <t>IGN 2, 4</t>
-  </si>
-  <si>
-    <t>IGN 1, 3</t>
-  </si>
-  <si>
     <t>RX</t>
   </si>
   <si>
@@ -781,6 +769,15 @@
   </si>
   <si>
     <t>Yes, but Lambda sensor needs to be connected to something else</t>
+  </si>
+  <si>
+    <t>IGN 1,3</t>
+  </si>
+  <si>
+    <t>IGN 2,4</t>
+  </si>
+  <si>
+    <t>VRIN2+</t>
   </si>
 </sst>
 </file>
@@ -1107,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1121,7 @@
     <col min="9" max="9" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="100.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
     <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.44140625" bestFit="1" customWidth="1"/>
@@ -1171,7 +1168,7 @@
         <v>128</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1215,7 +1212,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -1233,13 +1230,13 @@
         <v>130</v>
       </c>
       <c r="M3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1268,10 +1265,10 @@
         <v>131</v>
       </c>
       <c r="M4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1300,15 +1297,15 @@
         <v>131</v>
       </c>
       <c r="M5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -1320,22 +1317,22 @@
         <v>183</v>
       </c>
       <c r="L6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1355,19 +1352,19 @@
         <v>187</v>
       </c>
       <c r="M7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1396,10 +1393,10 @@
         <v>132</v>
       </c>
       <c r="M8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1422,13 +1419,13 @@
         <v>134</v>
       </c>
       <c r="M9" t="s">
+        <v>190</v>
+      </c>
+      <c r="N9" t="s">
         <v>191</v>
       </c>
-      <c r="N9" t="s">
-        <v>192</v>
-      </c>
       <c r="O9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1451,15 +1448,15 @@
         <v>133</v>
       </c>
       <c r="M10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -1474,18 +1471,18 @@
         <v>75</v>
       </c>
       <c r="L11" t="s">
+        <v>235</v>
+      </c>
+      <c r="M11" t="s">
+        <v>195</v>
+      </c>
+      <c r="O11" t="s">
         <v>237</v>
-      </c>
-      <c r="M11" t="s">
-        <v>196</v>
-      </c>
-      <c r="O11" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
@@ -1500,18 +1497,18 @@
         <v>75</v>
       </c>
       <c r="L12" t="s">
+        <v>236</v>
+      </c>
+      <c r="M12" t="s">
+        <v>195</v>
+      </c>
+      <c r="O12" t="s">
         <v>238</v>
-      </c>
-      <c r="M12" t="s">
-        <v>196</v>
-      </c>
-      <c r="O12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
@@ -1535,15 +1532,15 @@
         <v>136</v>
       </c>
       <c r="M13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
@@ -1567,15 +1564,15 @@
         <v>135</v>
       </c>
       <c r="M14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O14" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
@@ -1593,18 +1590,18 @@
         <v>137</v>
       </c>
       <c r="M15" t="s">
+        <v>190</v>
+      </c>
+      <c r="N15" t="s">
         <v>191</v>
       </c>
-      <c r="N15" t="s">
-        <v>192</v>
-      </c>
       <c r="O15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
@@ -1622,13 +1619,13 @@
         <v>138</v>
       </c>
       <c r="M16" t="s">
+        <v>190</v>
+      </c>
+      <c r="N16" t="s">
         <v>191</v>
       </c>
-      <c r="N16" t="s">
-        <v>192</v>
-      </c>
       <c r="O16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -1648,19 +1645,19 @@
         <v>139</v>
       </c>
       <c r="M17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -1680,19 +1677,19 @@
         <v>140</v>
       </c>
       <c r="M18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -1712,19 +1709,19 @@
         <v>140</v>
       </c>
       <c r="M19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -1765,10 +1762,10 @@
         <v>141</v>
       </c>
       <c r="M20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -1791,13 +1788,13 @@
         <v>142</v>
       </c>
       <c r="M21" t="s">
+        <v>190</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="O21" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -1820,10 +1817,10 @@
         <v>143</v>
       </c>
       <c r="M22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -1846,10 +1843,10 @@
         <v>144</v>
       </c>
       <c r="M23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -1872,10 +1869,10 @@
         <v>145</v>
       </c>
       <c r="M24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
@@ -1898,10 +1895,10 @@
         <v>146</v>
       </c>
       <c r="M25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
@@ -1924,15 +1921,15 @@
         <v>147</v>
       </c>
       <c r="M26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
@@ -1950,10 +1947,10 @@
         <v>148</v>
       </c>
       <c r="M27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -1982,7 +1979,7 @@
         <v>149</v>
       </c>
       <c r="M28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2002,19 +1999,19 @@
         <v>187</v>
       </c>
       <c r="M29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2034,19 +2031,19 @@
         <v>188</v>
       </c>
       <c r="M30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2066,19 +2063,19 @@
         <v>188</v>
       </c>
       <c r="M31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -2101,10 +2098,10 @@
         <v>151</v>
       </c>
       <c r="M32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -2127,10 +2124,10 @@
         <v>150</v>
       </c>
       <c r="M33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -2153,10 +2150,10 @@
         <v>152</v>
       </c>
       <c r="M34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -2179,13 +2176,13 @@
         <v>153</v>
       </c>
       <c r="M35" t="s">
+        <v>190</v>
+      </c>
+      <c r="N35" t="s">
         <v>191</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>192</v>
-      </c>
-      <c r="O35" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -2208,10 +2205,10 @@
         <v>154</v>
       </c>
       <c r="M36" t="s">
+        <v>190</v>
+      </c>
+      <c r="N36" t="s">
         <v>191</v>
-      </c>
-      <c r="N36" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -2234,10 +2231,10 @@
         <v>155</v>
       </c>
       <c r="M37" t="s">
+        <v>190</v>
+      </c>
+      <c r="N37" t="s">
         <v>191</v>
-      </c>
-      <c r="N37" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2260,10 +2257,10 @@
         <v>156</v>
       </c>
       <c r="M38" t="s">
+        <v>190</v>
+      </c>
+      <c r="N38" t="s">
         <v>191</v>
-      </c>
-      <c r="N38" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -2286,13 +2283,13 @@
         <v>158</v>
       </c>
       <c r="M39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N39" t="s">
+        <v>191</v>
+      </c>
+      <c r="O39" t="s">
         <v>192</v>
-      </c>
-      <c r="O39" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -2315,10 +2312,10 @@
         <v>157</v>
       </c>
       <c r="M40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -2353,7 +2350,7 @@
         <v>159</v>
       </c>
       <c r="M41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -2376,7 +2373,7 @@
         <v>160</v>
       </c>
       <c r="M42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -2399,7 +2396,7 @@
         <v>161</v>
       </c>
       <c r="M43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -2422,13 +2419,13 @@
         <v>162</v>
       </c>
       <c r="M44" t="s">
+        <v>190</v>
+      </c>
+      <c r="N44" t="s">
         <v>191</v>
       </c>
-      <c r="N44" t="s">
+      <c r="O44" t="s">
         <v>192</v>
-      </c>
-      <c r="O44" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -2466,16 +2463,16 @@
         <v>66</v>
       </c>
       <c r="L45" t="s">
+        <v>199</v>
+      </c>
+      <c r="M45" t="s">
         <v>200</v>
       </c>
-      <c r="M45" t="s">
-        <v>201</v>
-      </c>
       <c r="N45" t="s">
+        <v>191</v>
+      </c>
+      <c r="O45" t="s">
         <v>192</v>
-      </c>
-      <c r="O45" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -2498,10 +2495,10 @@
         <v>164</v>
       </c>
       <c r="M46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -2524,10 +2521,10 @@
         <v>163</v>
       </c>
       <c r="M47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -2550,10 +2547,10 @@
         <v>165</v>
       </c>
       <c r="M48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
@@ -2576,7 +2573,7 @@
         <v>166</v>
       </c>
       <c r="M49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -2599,10 +2596,10 @@
         <v>167</v>
       </c>
       <c r="M50" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -2625,10 +2622,10 @@
         <v>169</v>
       </c>
       <c r="M51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -2651,10 +2648,10 @@
         <v>168</v>
       </c>
       <c r="M52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -2677,7 +2674,7 @@
         <v>170</v>
       </c>
       <c r="O53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -2700,7 +2697,7 @@
         <v>171</v>
       </c>
       <c r="O54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -2723,10 +2720,10 @@
         <v>172</v>
       </c>
       <c r="M55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -2749,10 +2746,10 @@
         <v>172</v>
       </c>
       <c r="M56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -2775,7 +2772,7 @@
         <v>173</v>
       </c>
       <c r="M57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -2798,10 +2795,10 @@
         <v>174</v>
       </c>
       <c r="M58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -2824,10 +2821,10 @@
         <v>175</v>
       </c>
       <c r="M59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -2850,7 +2847,7 @@
         <v>176</v>
       </c>
       <c r="M60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -2870,7 +2867,7 @@
         <v>66</v>
       </c>
       <c r="F61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -2879,7 +2876,7 @@
         <v>177</v>
       </c>
       <c r="M61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -2899,10 +2896,10 @@
         <v>66</v>
       </c>
       <c r="L62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -2925,7 +2922,7 @@
         <v>179</v>
       </c>
       <c r="M63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -2948,7 +2945,7 @@
         <v>178</v>
       </c>
       <c r="M64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
@@ -2971,7 +2968,7 @@
         <v>180</v>
       </c>
       <c r="M65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
@@ -2991,10 +2988,10 @@
         <v>181</v>
       </c>
       <c r="M66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
@@ -3011,13 +3008,13 @@
         <v>181</v>
       </c>
       <c r="M67" t="s">
+        <v>190</v>
+      </c>
+      <c r="N67" t="s">
         <v>191</v>
       </c>
-      <c r="N67" t="s">
-        <v>192</v>
-      </c>
       <c r="O67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
@@ -3037,7 +3034,7 @@
         <v>181</v>
       </c>
       <c r="M68" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -3060,10 +3057,10 @@
         <v>181</v>
       </c>
       <c r="M69" t="s">
+        <v>190</v>
+      </c>
+      <c r="N69" t="s">
         <v>191</v>
-      </c>
-      <c r="N69" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
@@ -3083,10 +3080,10 @@
         <v>181</v>
       </c>
       <c r="M70" t="s">
+        <v>190</v>
+      </c>
+      <c r="N70" t="s">
         <v>191</v>
-      </c>
-      <c r="N70" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -3103,10 +3100,10 @@
         <v>181</v>
       </c>
       <c r="M71" t="s">
+        <v>190</v>
+      </c>
+      <c r="N71" t="s">
         <v>191</v>
-      </c>
-      <c r="N71" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -3126,18 +3123,18 @@
         <v>181</v>
       </c>
       <c r="M72" t="s">
+        <v>190</v>
+      </c>
+      <c r="N72" t="s">
         <v>191</v>
       </c>
-      <c r="N72" t="s">
+      <c r="O72" t="s">
         <v>192</v>
-      </c>
-      <c r="O72" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
         <v>108</v>
@@ -3146,24 +3143,24 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E73" t="s">
         <v>66</v>
       </c>
       <c r="L73" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
         <v>108</v>
@@ -3172,24 +3169,24 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E74" t="s">
         <v>66</v>
       </c>
       <c r="L74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M74" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
         <v>108</v>
@@ -3198,24 +3195,24 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E75" t="s">
         <v>66</v>
       </c>
       <c r="L75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B76" t="s">
         <v>108</v>
@@ -3224,24 +3221,24 @@
         <v>4</v>
       </c>
       <c r="D76" t="s">
+        <v>216</v>
+      </c>
+      <c r="E76" t="s">
+        <v>66</v>
+      </c>
+      <c r="L76" t="s">
         <v>217</v>
       </c>
-      <c r="E76" t="s">
-        <v>66</v>
-      </c>
-      <c r="L76" t="s">
-        <v>218</v>
-      </c>
       <c r="M76" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
         <v>108</v>
@@ -3250,24 +3247,24 @@
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E77" t="s">
         <v>66</v>
       </c>
       <c r="L77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M77" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B78" t="s">
         <v>108</v>
@@ -3276,44 +3273,44 @@
         <v>13</v>
       </c>
       <c r="D78" t="s">
+        <v>214</v>
+      </c>
+      <c r="E78" t="s">
+        <v>66</v>
+      </c>
+      <c r="L78" t="s">
         <v>215</v>
       </c>
-      <c r="E78" t="s">
-        <v>66</v>
-      </c>
-      <c r="L78" t="s">
-        <v>216</v>
-      </c>
       <c r="M78" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O78" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C79">
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>102</v>
       </c>
       <c r="L79" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>